<commit_message>
Update the whole file
</commit_message>
<xml_diff>
--- a/input/comp_mrs_db_cat.xlsx
+++ b/input/comp_mrs_db_cat.xlsx
@@ -681,7 +681,7 @@
         <v>-0.02253571108019671</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.349324843968644</v>
+        <v>1.331617765164322</v>
       </c>
       <c r="AE2" t="n">
         <v>-10.71287134363504</v>
@@ -781,7 +781,7 @@
         <v>0.05145483745961987</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.1790125063937677</v>
+        <v>0.1615255895249083</v>
       </c>
       <c r="AE3" t="n">
         <v>-14.58010571514267</v>
@@ -881,7 +881,7 @@
         <v>-0.02311568454788574</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.3251491368039667</v>
+        <v>-0.2190164776938517</v>
       </c>
       <c r="AE4" t="n">
         <v>-10.59408744031139</v>
@@ -981,7 +981,7 @@
         <v>-0.03391007751123196</v>
       </c>
       <c r="AD5" t="n">
-        <v>1.295364897130082</v>
+        <v>1.247005318008205</v>
       </c>
       <c r="AE5" t="n">
         <v>-10.19873570115378</v>
@@ -1181,7 +1181,7 @@
         <v>0.01656407546583211</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.6643901723454653</v>
+        <v>0.6325998303579028</v>
       </c>
       <c r="AE7" t="n">
         <v>-12.52251865458284</v>
@@ -1281,7 +1281,7 @@
         <v>0.03658320797548056</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.0154326596133041</v>
+        <v>0.01465343221456516</v>
       </c>
       <c r="AE8" t="n">
         <v>-15.0921182512653</v>
@@ -1381,7 +1381,7 @@
         <v>-0.0257802155774243</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.5184410162249959</v>
+        <v>0.2522790160453459</v>
       </c>
       <c r="AE9" t="n">
         <v>-12.25232032141117</v>
@@ -1481,7 +1481,7 @@
         <v>-0.02989159533577808</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.3700482611681618</v>
+        <v>0.3692449490957154</v>
       </c>
       <c r="AE10" t="n">
         <v>-13.43421122439342</v>
@@ -1581,7 +1581,7 @@
         <v>0.005491268636792317</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.2454642123782856</v>
+        <v>0.2401404958660949</v>
       </c>
       <c r="AE11" t="n">
         <v>-11.93731123504216</v>
@@ -1681,7 +1681,7 @@
         <v>0.0860694672710957</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.05169514222383378</v>
+        <v>0.04541607648193594</v>
       </c>
       <c r="AE12" t="n">
         <v>-11.69034257985</v>
@@ -1781,7 +1781,7 @@
         <v>-0.01425994787852184</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.3448120709288106</v>
+        <v>0.3439855200790409</v>
       </c>
       <c r="AE13" t="n">
         <v>-12.74396681066839</v>
@@ -1881,7 +1881,7 @@
         <v>0.01950246349247608</v>
       </c>
       <c r="AD14" t="n">
-        <v>-0.2366090168519545</v>
+        <v>-0.2771027461821775</v>
       </c>
       <c r="AE14" t="n">
         <v>-9.882164425305898</v>
@@ -1981,7 +1981,7 @@
         <v>-0.08801296918238558</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.9464072142749296</v>
+        <v>0.9423268497684154</v>
       </c>
       <c r="AE15" t="n">
         <v>-11.80059150596449</v>
@@ -2181,7 +2181,7 @@
         <v>0.01266755913370944</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.4999581114549639</v>
+        <v>0.4934238596771008</v>
       </c>
       <c r="AE17" t="n">
         <v>-15.37674820929016</v>
@@ -2281,7 +2281,7 @@
         <v>-0.1048208634132849</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.1833057836558002</v>
+        <v>0.1819533668932887</v>
       </c>
       <c r="AE18" t="n">
         <v>-13.42280115001057</v>
@@ -2381,7 +2381,7 @@
         <v>0.01469753701812776</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.1283109762246061</v>
+        <v>0.1274835671478239</v>
       </c>
       <c r="AE19" t="n">
         <v>-12.11501624570678</v>
@@ -2581,7 +2581,7 @@
         <v>0.06652481685425474</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.12262271326239</v>
+        <v>0.1175831222413791</v>
       </c>
       <c r="AE21" t="n">
         <v>-13.21489960443659</v>
@@ -2681,7 +2681,7 @@
         <v>-0.01791581281148704</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.08755629789200478</v>
+        <v>0.08567806172022781</v>
       </c>
       <c r="AE22" t="n">
         <v>-12.23345658516506</v>
@@ -2781,7 +2781,7 @@
         <v>-0.01723232483948973</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.2539916717785259</v>
+        <v>0.2472168566298102</v>
       </c>
       <c r="AE23" t="n">
         <v>-11.5992000271969</v>
@@ -2881,7 +2881,7 @@
         <v>0.02140151786384475</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.9667243371685512</v>
+        <v>0.9657324797925104</v>
       </c>
       <c r="AE24" t="n">
         <v>-11.46661957331528</v>
@@ -2981,7 +2981,7 @@
         <v>-0.1252764488401676</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.8735024107446513</v>
+        <v>0.6240851513992403</v>
       </c>
       <c r="AE25" t="n">
         <v>-9.98027283460573</v>
@@ -3081,7 +3081,7 @@
         <v>-0.005562017600533308</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.6485321294332147</v>
+        <v>0.6257639271635584</v>
       </c>
       <c r="AE26" t="n">
         <v>-14.51851968851755</v>
@@ -3181,7 +3181,7 @@
         <v>-0.004944895094070909</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.7147900127387261</v>
+        <v>0.7119843018245802</v>
       </c>
       <c r="AE27" t="n">
         <v>-12.01886751273979</v>
@@ -3281,7 +3281,7 @@
         <v>-0.0566012107196378</v>
       </c>
       <c r="AD28" t="n">
-        <v>1.21651060392319</v>
+        <v>1.214379302193214</v>
       </c>
       <c r="AE28" t="n">
         <v>-15.37167225364937</v>
@@ -3381,7 +3381,7 @@
         <v>-0.1544274508518571</v>
       </c>
       <c r="AD29" t="n">
-        <v>-0.101395378449396</v>
+        <v>-0.2762158054446322</v>
       </c>
       <c r="AE29" t="n">
         <v>-13.5241701207883</v>
@@ -3481,7 +3481,7 @@
         <v>-0.01375837472189369</v>
       </c>
       <c r="AD30" t="n">
-        <v>-1.28158685972077</v>
+        <v>-1.416062347784709</v>
       </c>
       <c r="AE30" t="n">
         <v>-11.49508205430502</v>
@@ -3581,7 +3581,7 @@
         <v>-0.09324834772141333</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.7571054089102038</v>
+        <v>0.6333022396118085</v>
       </c>
       <c r="AE31" t="n">
         <v>-13.10995632210551</v>
@@ -3681,7 +3681,7 @@
         <v>-0.03038792594645022</v>
       </c>
       <c r="AD32" t="n">
-        <v>-0.7800801661261121</v>
+        <v>-1.029959203170345</v>
       </c>
       <c r="AE32" t="n">
         <v>-12.15714777458812</v>
@@ -3781,7 +3781,7 @@
         <v>0.01458613964633884</v>
       </c>
       <c r="AD33" t="n">
-        <v>0.6688358936231841</v>
+        <v>0.6096467109995476</v>
       </c>
       <c r="AE33" t="n">
         <v>-12.95483354674426</v>
@@ -3881,7 +3881,7 @@
         <v>-0.01172553878460611</v>
       </c>
       <c r="AD34" t="n">
-        <v>0.2036337351286908</v>
+        <v>0.160715332494081</v>
       </c>
       <c r="AE34" t="n">
         <v>-11.43590039691728</v>
@@ -3981,7 +3981,7 @@
         <v>-0.01210242488285608</v>
       </c>
       <c r="AD35" t="n">
-        <v>0.7926442020663729</v>
+        <v>0.7917059169459646</v>
       </c>
       <c r="AE35" t="n">
         <v>-13.36936733974361</v>
@@ -4181,7 +4181,7 @@
         <v>0.07903386814482644</v>
       </c>
       <c r="AD37" t="n">
-        <v>-0.006684037700948771</v>
+        <v>-0.01968783795405432</v>
       </c>
       <c r="AE37" t="n">
         <v>-12.66543848325756</v>
@@ -4681,7 +4681,7 @@
         <v>-0.1240316426625881</v>
       </c>
       <c r="AD42" t="n">
-        <v>0.5120571413802395</v>
+        <v>0.492203158203061</v>
       </c>
       <c r="AE42" t="n">
         <v>-13.7896516881348</v>
@@ -4781,7 +4781,7 @@
         <v>-0.03817945356419498</v>
       </c>
       <c r="AD43" t="n">
-        <v>1.171238522772072</v>
+        <v>1.166045041745317</v>
       </c>
       <c r="AE43" t="n">
         <v>-12.91365853710254</v>
@@ -4881,7 +4881,7 @@
         <v>0.03989310575973623</v>
       </c>
       <c r="AD44" t="n">
-        <v>0.04952614163671054</v>
+        <v>0.03885572782721866</v>
       </c>
       <c r="AE44" t="n">
         <v>-12.58299944621622</v>
@@ -5081,7 +5081,7 @@
         <v>0.04526844422307467</v>
       </c>
       <c r="AD46" t="n">
-        <v>0.6797772062528168</v>
+        <v>0.6781037513389003</v>
       </c>
       <c r="AE46" t="n">
         <v>-14.02068089885143</v>
@@ -5181,7 +5181,7 @@
         <v>-0.08771332036010683</v>
       </c>
       <c r="AD47" t="n">
-        <v>0.3458254045777432</v>
+        <v>0.3439146509921893</v>
       </c>
       <c r="AE47" t="n">
         <v>-13.76433087242771</v>
@@ -5281,7 +5281,7 @@
         <v>0.01171826334382941</v>
       </c>
       <c r="AD48" t="n">
-        <v>0.02688030345492576</v>
+        <v>-0.00429677831595654</v>
       </c>
       <c r="AE48" t="n">
         <v>-13.58696023262923</v>
@@ -5481,7 +5481,7 @@
         <v>-0.1035686816929112</v>
       </c>
       <c r="AD50" t="n">
-        <v>0.6863028741057466</v>
+        <v>0.6832196971504075</v>
       </c>
       <c r="AE50" t="n">
         <v>-11.06433018238832</v>
@@ -5581,7 +5581,7 @@
         <v>0.01446724075091104</v>
       </c>
       <c r="AD51" t="n">
-        <v>0.1862437341284388</v>
+        <v>-0.03057912132167632</v>
       </c>
       <c r="AE51" t="n">
         <v>-9.811596911047625</v>
@@ -5681,7 +5681,7 @@
         <v>-0.05476918884983398</v>
       </c>
       <c r="AD52" t="n">
-        <v>0.4312064758209718</v>
+        <v>0.4212951720538849</v>
       </c>
       <c r="AE52" t="n">
         <v>-12.52304508827194</v>
@@ -5781,7 +5781,7 @@
         <v>-0.1476485834892379</v>
       </c>
       <c r="AD53" t="n">
-        <v>-0.1276147424478848</v>
+        <v>-0.1357650071055301</v>
       </c>
       <c r="AE53" t="n">
         <v>-11.3042439117639</v>
@@ -5881,7 +5881,7 @@
         <v>0.07631202673319253</v>
       </c>
       <c r="AD54" t="n">
-        <v>0.04464194872250103</v>
+        <v>-0.0347585287505181</v>
       </c>
       <c r="AE54" t="n">
         <v>-10.95383022351939</v>
@@ -5981,7 +5981,7 @@
         <v>-0.1023596181889312</v>
       </c>
       <c r="AD55" t="n">
-        <v>0.06375664783978777</v>
+        <v>0.05214779532647944</v>
       </c>
       <c r="AE55" t="n">
         <v>-12.69528876072049</v>
@@ -6081,7 +6081,7 @@
         <v>0.1065500901464023</v>
       </c>
       <c r="AD56" t="n">
-        <v>-0.02842617464579093</v>
+        <v>-0.274777650061912</v>
       </c>
       <c r="AE56" t="n">
         <v>-11.47293217579436</v>
@@ -6181,7 +6181,7 @@
         <v>-0.006678942190835382</v>
       </c>
       <c r="AD57" t="n">
-        <v>0.1535286260219229</v>
+        <v>0.1493591001217888</v>
       </c>
       <c r="AE57" t="n">
         <v>-11.13192123878857</v>
@@ -6281,7 +6281,7 @@
         <v>0.07808724506113843</v>
       </c>
       <c r="AD58" t="n">
-        <v>-0.002499888651234683</v>
+        <v>-0.5265188872074642</v>
       </c>
       <c r="AE58" t="n">
         <v>-11.28390573792729</v>
@@ -6381,7 +6381,7 @@
         <v>-0.02650926173246486</v>
       </c>
       <c r="AD59" t="n">
-        <v>-0.651592177382373</v>
+        <v>-0.6537420480262576</v>
       </c>
       <c r="AE59" t="n">
         <v>-13.60755576729628</v>
@@ -6481,7 +6481,7 @@
         <v>0.01581699255595311</v>
       </c>
       <c r="AD60" t="n">
-        <v>0.1918172034293323</v>
+        <v>0.1895020719705186</v>
       </c>
       <c r="AE60" t="n">
         <v>-13.11686081229195</v>

</xml_diff>